<commit_message>
Created new functions parsing_edgetimes_excel, had to modify the excel too.
</commit_message>
<xml_diff>
--- a/excel/EmergencyProcess_EdgeTimes.xlsx
+++ b/excel/EmergencyProcess_EdgeTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC5A811-017B-4390-BE1C-CAA79F38CBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02CC4A6-009B-45F9-ABC7-60170B2C2DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
   </bookViews>
   <sheets>
     <sheet name="test_times_a" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
   <si>
     <t>Time with units</t>
   </si>
@@ -233,10 +233,13 @@
     <t>Transport continues (ambulance/doctor changes vehicle)</t>
   </si>
   <si>
-    <t>Transport continues (ambulance +doctor)</t>
-  </si>
-  <si>
     <t>Transport continues (helicopter)</t>
+  </si>
+  <si>
+    <t>Transport continues (ambulance + doctor)</t>
+  </si>
+  <si>
+    <t>Helicopter leaving the base</t>
   </si>
 </sst>
 </file>
@@ -599,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71562E14-3918-4016-8B89-2022C6498FB8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,7 +844,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
@@ -932,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F147F0-D3D6-463F-9496-D7B453D285B9}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1284,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A27481-A897-4478-B9B6-2FE8DCB74316}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1611,7 +1614,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -1625,7 +1628,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Calculator works, had to modify Excel to do so
</commit_message>
<xml_diff>
--- a/excel/EmergencyProcess_EdgeTimes.xlsx
+++ b/excel/EmergencyProcess_EdgeTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02CC4A6-009B-45F9-ABC7-60170B2C2DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA978AB-8141-4916-AF36-3707E09F7FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>Infusion starts --&gt; Packing</t>
   </si>
   <si>
-    <t>Ambulance leaving scene --&gt; Doctor changes vehicle</t>
-  </si>
-  <si>
     <t>Ambulance leaving the scene --&gt; At hospital</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Infusion starts</t>
   </si>
   <si>
-    <t>Ambulance leaving scene</t>
-  </si>
-  <si>
     <t>Transport continues</t>
   </si>
   <si>
@@ -240,6 +234,12 @@
   </si>
   <si>
     <t>Helicopter leaving the base</t>
+  </si>
+  <si>
+    <t>Ambulance and doctor leaving the scene</t>
+  </si>
+  <si>
+    <t>Ambulance and doctor leaving</t>
   </si>
 </sst>
 </file>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71562E14-3918-4016-8B89-2022C6498FB8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,25 +617,25 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -662,10 +662,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -676,10 +676,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -704,10 +704,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -718,10 +718,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -732,10 +732,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -760,10 +760,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -774,10 +774,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -788,10 +788,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -816,10 +816,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -830,10 +830,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -858,10 +858,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -872,10 +872,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24">
         <v>20</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -900,10 +900,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -914,10 +914,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -936,7 +936,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -954,10 +954,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -973,7 +973,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -989,7 +989,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1043,7 +1043,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1051,7 +1051,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1066,33 +1066,33 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1128,7 +1128,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1147,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1155,7 +1155,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1163,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1184,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1220,7 +1220,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1301,24 +1301,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1357,10 +1357,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1371,10 +1371,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1469,10 +1469,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1497,10 +1497,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1511,10 +1511,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1600,10 +1600,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
         <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
       </c>
       <c r="C33">
         <v>1</v>

</xml_diff>

<commit_message>
Calculator works for chart B, modified that sheet in excel too
</commit_message>
<xml_diff>
--- a/excel/EmergencyProcess_EdgeTimes.xlsx
+++ b/excel/EmergencyProcess_EdgeTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA978AB-8141-4916-AF36-3707E09F7FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742ED166-50A7-4C2A-AE26-20F058F4379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
   </bookViews>
   <sheets>
     <sheet name="test_times_a" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="65">
   <si>
     <t>Time with units</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Ambulance leaving</t>
   </si>
   <si>
-    <t>Ambulance + doctor leaving</t>
-  </si>
-  <si>
     <t>Helicopter leaving</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Ambulance leaving the scene</t>
   </si>
   <si>
-    <t>Ambulance + doctor leaving the scene</t>
-  </si>
-  <si>
     <t>Helicopter leaving the scene</t>
   </si>
   <si>
@@ -221,18 +215,6 @@
     <t>Infusion starts</t>
   </si>
   <si>
-    <t>Transport continues</t>
-  </si>
-  <si>
-    <t>Transport continues (ambulance/doctor changes vehicle)</t>
-  </si>
-  <si>
-    <t>Transport continues (helicopter)</t>
-  </si>
-  <si>
-    <t>Transport continues (ambulance + doctor)</t>
-  </si>
-  <si>
     <t>Helicopter leaving the base</t>
   </si>
   <si>
@@ -240,6 +222,15 @@
   </si>
   <si>
     <t>Ambulance and doctor leaving</t>
+  </si>
+  <si>
+    <t>Transport continues in Ambulance</t>
+  </si>
+  <si>
+    <t>Transport continues in Ambulance and doctor</t>
+  </si>
+  <si>
+    <t>Transport continues in Helicopter</t>
   </si>
 </sst>
 </file>
@@ -602,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71562E14-3918-4016-8B89-2022C6498FB8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -632,7 +623,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -647,10 +638,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -662,10 +653,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -676,10 +667,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -693,7 +684,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -704,10 +695,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -718,10 +709,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -732,10 +723,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -746,10 +737,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -760,10 +751,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -774,10 +765,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -788,10 +779,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -802,10 +793,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -816,10 +807,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -830,10 +821,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -844,10 +835,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -858,10 +849,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -872,10 +863,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <v>20</v>
@@ -886,10 +877,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -900,10 +891,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -914,10 +905,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1285,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A27481-A897-4478-B9B6-2FE8DCB74316}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1315,7 +1306,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -1329,10 +1320,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1343,10 +1334,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1357,10 +1348,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1374,7 +1365,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -1385,10 +1376,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1399,10 +1390,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -1413,10 +1404,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -1427,10 +1418,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1441,10 +1432,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1455,10 +1446,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1469,10 +1460,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1483,10 +1474,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1497,10 +1488,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1511,10 +1502,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1525,10 +1516,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1539,10 +1530,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -1553,10 +1544,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1567,10 +1558,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1586,10 +1577,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1598,59 +1589,91 @@
         <v>5</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5</v>
+      </c>
+    </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29">
-        <v>10</v>
-      </c>
-      <c r="D29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30">
-        <v>10</v>
-      </c>
-      <c r="D30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33">
         <v>5</v>
       </c>
-      <c r="D31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
       <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parsing works but is too complicated. Added probabilities to Excel
</commit_message>
<xml_diff>
--- a/excel/EmergencyProcess_EdgeTimes.xlsx
+++ b/excel/EmergencyProcess_EdgeTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742ED166-50A7-4C2A-AE26-20F058F4379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA4AAF3-3D7C-4677-BE0D-04C5367EBBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
   </bookViews>
   <sheets>
     <sheet name="test_times_a" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>Time with units</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Transport continues in Helicopter</t>
+  </si>
+  <si>
+    <t>probability</t>
   </si>
 </sst>
 </file>
@@ -593,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71562E14-3918-4016-8B89-2022C6498FB8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -619,7 +622,9 @@
       <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -634,7 +639,9 @@
       <c r="D2">
         <v>1.5</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -649,7 +656,9 @@
       <c r="D3">
         <v>1.5</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -664,6 +673,9 @@
       <c r="D4">
         <v>5</v>
       </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -678,6 +690,9 @@
       <c r="D5">
         <v>1.5</v>
       </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -692,6 +707,9 @@
       <c r="D7">
         <v>40</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -706,6 +724,9 @@
       <c r="D8">
         <v>40</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -720,6 +741,9 @@
       <c r="D9" s="1">
         <v>20</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -734,6 +758,9 @@
       <c r="D10" s="1">
         <v>40</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -748,6 +775,9 @@
       <c r="D12">
         <v>10</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -762,6 +792,9 @@
       <c r="D13">
         <v>20</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -776,6 +809,9 @@
       <c r="D14">
         <v>5</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -790,8 +826,11 @@
       <c r="D16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -804,8 +843,11 @@
       <c r="D17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -818,8 +860,11 @@
       <c r="D18">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -832,8 +877,11 @@
       <c r="D20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -846,8 +894,11 @@
       <c r="D21">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -860,8 +911,11 @@
       <c r="D23">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -874,8 +928,11 @@
       <c r="D24">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -888,8 +945,11 @@
       <c r="D25" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -902,8 +962,11 @@
       <c r="D26" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -915,6 +978,9 @@
       </c>
       <c r="D28">
         <v>10</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +993,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1276,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A27481-A897-4478-B9B6-2FE8DCB74316}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1290,7 +1356,7 @@
     <col min="4" max="4" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -1303,8 +1369,11 @@
       <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1317,8 +1386,11 @@
       <c r="D2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1331,8 +1403,11 @@
       <c r="D3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1345,8 +1420,11 @@
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1359,8 +1437,11 @@
       <c r="D5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1373,8 +1454,11 @@
       <c r="D7">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1387,8 +1471,11 @@
       <c r="D8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1401,8 +1488,11 @@
       <c r="D9" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1415,8 +1505,11 @@
       <c r="D10" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1429,8 +1522,11 @@
       <c r="D12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1443,8 +1539,11 @@
       <c r="D13">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1457,8 +1556,11 @@
       <c r="D15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1471,8 +1573,11 @@
       <c r="D16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1485,8 +1590,11 @@
       <c r="D17">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1499,8 +1607,11 @@
       <c r="D19" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1513,8 +1624,11 @@
       <c r="D20">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1527,8 +1641,11 @@
       <c r="D22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1541,8 +1658,11 @@
       <c r="D23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1555,8 +1675,11 @@
       <c r="D24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -1569,13 +1692,16 @@
       <c r="D25" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1588,8 +1714,11 @@
       <c r="D27" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1602,8 +1731,11 @@
       <c r="D28" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1616,12 +1748,15 @@
       <c r="D29" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
@@ -1634,8 +1769,11 @@
       <c r="D31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>63</v>
       </c>
@@ -1648,8 +1786,11 @@
       <c r="D32">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -1662,8 +1803,11 @@
       <c r="D33">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1675,6 +1819,9 @@
       </c>
       <c r="D35">
         <v>10</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excels, added probabilities
</commit_message>
<xml_diff>
--- a/excel/EmergencyProcess_EdgeTimes.xlsx
+++ b/excel/EmergencyProcess_EdgeTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA4AAF3-3D7C-4677-BE0D-04C5367EBBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FB8A27-8A94-4C63-B4C6-B5AB10A8B22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C67DC1AD-9262-44FA-852C-0E07C84D8313}"/>
   </bookViews>
   <sheets>
     <sheet name="test_times_a" sheetId="4" r:id="rId1"/>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71562E14-3918-4016-8B89-2022C6498FB8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,7 +912,7 @@
         <v>40</v>
       </c>
       <c r="E23">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A27481-A897-4478-B9B6-2FE8DCB74316}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1642,7 +1642,7 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>